<commit_message>
add corr table, update wilcox and permanvoa table
</commit_message>
<xml_diff>
--- a/table/env_corr.xlsx
+++ b/table/env_corr.xlsx
@@ -371,92 +371,92 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Temp</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Sal</t>
+          <t>Salinity</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sigma*theta</t>
+          <t>SigmaTheta</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Den</t>
+          <t>Density</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Oxy</t>
+          <t>Oxygen</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Fluo</t>
+          <t>Fluorescence</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Trans</t>
+          <t>Transmission</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Sand</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Silt</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Clay</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>D50</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Clay</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Silt</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Sand</t>
-        </is>
-      </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>TOC</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>TOC</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>TN</t>
-        </is>
-      </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>delta13C</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Chla</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>WC</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>delta^13*C</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Chla</t>
-        </is>
-      </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Por</t>
+          <t>Porosity</t>
         </is>
       </c>
     </row>
@@ -716,92 +716,92 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Temp</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Sal</t>
+          <t>Salinity</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sigma*theta</t>
+          <t>SigmaTheta</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Den</t>
+          <t>Density</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Oxy</t>
+          <t>Oxygen</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Fluo</t>
+          <t>Fluorescence</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Trans</t>
+          <t>Transmission</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Sand</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Silt</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Clay</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>D50</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Clay</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Silt</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Sand</t>
-        </is>
-      </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>TOC</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>TOC</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>TN</t>
-        </is>
-      </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>delta13C</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Chla</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>WC</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>delta^13*C</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Chla</t>
-        </is>
-      </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Por</t>
+          <t>Porosity</t>
         </is>
       </c>
     </row>

</xml_diff>